<commit_message>
Addition of demo tour
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\git\AccountCreation\NewAccount\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39F2935E-4067-4550-B065-CE2BB04767B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D71FD1D9-8245-4501-BA97-7BB46F37F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" sheetId="3" r:id="rId1"/>
     <sheet name="ContactUs" sheetId="4" r:id="rId2"/>
+    <sheet name="createNewAccount" sheetId="5" r:id="rId3"/>
+    <sheet name="Registration" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Flag</t>
   </si>
@@ -110,6 +114,12 @@
   </si>
   <si>
     <t>Customer service</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>TC01</t>
   </si>
 </sst>
 </file>
@@ -133,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,12 +191,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9B31E8-AA30-4D24-867C-0200B0B0BF91}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -591,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E05829-DD67-4E48-986B-1C42B616DD59}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,4 +646,61 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2659DC28-B26F-47CB-8F35-D1E6BD87A146}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C529E7-D62F-4EF1-B4A9-C6F81D5D2ABB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Registration Page and Functions
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26019"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\git\AccountCreation\NewAccount\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D71FD1D9-8245-4501-BA97-7BB46F37F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77FB995F-6275-4C4E-B406-4A3646C90B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Flag</t>
   </si>
@@ -119,7 +119,52 @@
     <t>TestCaseName</t>
   </si>
   <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
     <t>TC01</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>7761237786</t>
+  </si>
+  <si>
+    <t>raj_sharma@email.com</t>
+  </si>
+  <si>
+    <t>1506, VeteranPkway</t>
+  </si>
+  <si>
+    <t>Macon</t>
+  </si>
+  <si>
+    <t>31670</t>
+  </si>
+  <si>
+    <t>UNITED STATES</t>
+  </si>
+  <si>
+    <t>raj_sharma</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
   </si>
 </sst>
 </file>
@@ -191,13 +236,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9B31E8-AA30-4D24-867C-0200B0B0BF91}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -673,34 +720,115 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C529E7-D62F-4EF1-B4A9-C6F81D5D2ABB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{BEEC4FDB-D72D-4ADA-8D94-F9795C724318}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of Flight Page
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\git\AccountCreation\NewAccount\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77FB995F-6275-4C4E-B406-4A3646C90B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{B6929EE2-DBA5-4559-98F4-3CB8F3EECC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF3F8EB-6F83-407C-9AF0-4293C42630E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="ContactUs" sheetId="4" r:id="rId2"/>
     <sheet name="createNewAccount" sheetId="5" r:id="rId3"/>
     <sheet name="Registration" sheetId="6" r:id="rId4"/>
+    <sheet name="Flights" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Flag</t>
   </si>
@@ -137,7 +138,7 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>TC01</t>
+    <t>TC01_Registration</t>
   </si>
   <si>
     <t>Raj</t>
@@ -165,6 +166,9 @@
   </si>
   <si>
     <t>Welcome@123</t>
+  </si>
+  <si>
+    <t>TC01_Flights</t>
   </si>
 </sst>
 </file>
@@ -723,7 +727,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,4 +835,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6AA1CA-87B0-47A4-AE50-B42828B03339}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>